<commit_message>
Config test cases updated
</commit_message>
<xml_diff>
--- a/testdata/test_cases.xlsx
+++ b/testdata/test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DiagonalStuff\test-aryabhat\Automated_testing\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8B8E6B-DD29-4273-A560-C14128AFACAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AA2A03-C754-40FB-80AB-0252F92887A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{E4B8BAA6-053C-490B-8A8F-CDABAC5CBC80}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E4B8BAA6-053C-490B-8A8F-CDABAC5CBC80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="990">
   <si>
     <t>Test_ID</t>
   </si>
@@ -3230,9 +3230,6 @@
     <t>{"provider_name": "llm_provider_name", "user_id": "valid_userId", "apikey": "valid_apikey", "api_proxy_address": "valid_proxy", "is_enabled": false, "created_at": "llm_created_at", "temperature": valid_temperature }</t>
   </si>
   <si>
-    <t>{"tag_id": "invalid_tag_id", "tag_name":"invalid_tag_name", "modified_by":"valid_userId"}</t>
-  </si>
-  <si>
     <t>{"tag_id": "invalid_tag_id", "tag_name":"Machine Learning", "modified_by":"valid_userId"}</t>
   </si>
   <si>
@@ -3308,13 +3305,16 @@
     <t>{"user_id": "valid_userId", "chat_id": "valid_chat_id", "message_ids": "valid_message_id", "is_RL": false, "is_liked": 1}</t>
   </si>
   <si>
-    <t>{"model_id": "valid_model_id", "provider_id": "valid_provider_id", "chat_id": "valid_chat_id", "user_input": "valid_user_input", "user_id": "valid_userId", "department_tag": "valid_dept_tag"}</t>
-  </si>
-  <si>
     <t>{"chat_id": "{{TC11A01.Notebook_id}}"}</t>
   </si>
   <si>
     <t>Create LLM with invalid user ID</t>
+  </si>
+  <si>
+    <t>{"tag_id": "68x4x44x8xxx409f3xx8x6x2", "tag_name": "rename_tag", "modified_by": "valid_userId"}</t>
+  </si>
+  <si>
+    <t>{"Model_id": "valid_model_id", "Provider_id": "valid_provider_id", "Chat_id": "valid_chat_id", "User_input": "valid_user_input", "User_id": "valid_userId", "Department_tag": "valid_dept_tag"}</t>
   </si>
 </sst>
 </file>
@@ -3707,14 +3707,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB1F54A-02EF-463F-B588-F0453A90B53E}">
   <dimension ref="A1:O259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="101" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G180" sqref="G180"/>
+    <sheetView tabSelected="1" topLeftCell="C215" zoomScale="160" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.109375" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
@@ -3788,7 +3788,7 @@
         <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="J2">
         <v>200</v>
@@ -3820,7 +3820,7 @@
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="J3">
         <v>401</v>
@@ -3890,7 +3890,7 @@
         <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="J5">
         <v>415</v>
@@ -5753,9 +5753,6 @@
       <c r="E61" t="s">
         <v>61</v>
       </c>
-      <c r="F61" t="s">
-        <v>774</v>
-      </c>
       <c r="H61" t="s">
         <v>858</v>
       </c>
@@ -5978,7 +5975,7 @@
         <v>18</v>
       </c>
       <c r="H68" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="J68">
         <v>422</v>
@@ -6106,7 +6103,7 @@
         <v>18</v>
       </c>
       <c r="H72" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="J72">
         <v>422</v>
@@ -6135,7 +6132,7 @@
         <v>18</v>
       </c>
       <c r="H73" t="s">
-        <v>961</v>
+        <v>988</v>
       </c>
       <c r="J73">
         <v>404</v>
@@ -6161,7 +6158,7 @@
         <v>94</v>
       </c>
       <c r="H74" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="J74">
         <v>403</v>
@@ -6487,7 +6484,7 @@
         <v>18</v>
       </c>
       <c r="H84" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="J84">
         <v>200</v>
@@ -6519,7 +6516,7 @@
         <v>18</v>
       </c>
       <c r="H85" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="J85">
         <v>422</v>
@@ -6580,7 +6577,7 @@
         <v>693</v>
       </c>
       <c r="H87" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="J87">
         <v>401</v>
@@ -6612,7 +6609,7 @@
         <v>18</v>
       </c>
       <c r="H88" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="J88">
         <v>200</v>
@@ -6888,7 +6885,7 @@
         <v>18</v>
       </c>
       <c r="H97" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="J97">
         <v>200</v>
@@ -6920,7 +6917,7 @@
         <v>18</v>
       </c>
       <c r="H98" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="J98">
         <v>422</v>
@@ -6952,7 +6949,7 @@
         <v>18</v>
       </c>
       <c r="H99" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="J99">
         <v>202</v>
@@ -6987,7 +6984,7 @@
         <v>18</v>
       </c>
       <c r="H100" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="J100">
         <v>422</v>
@@ -7019,7 +7016,7 @@
         <v>18</v>
       </c>
       <c r="H101" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="J101">
         <v>422</v>
@@ -7170,7 +7167,7 @@
         <v>79</v>
       </c>
       <c r="E106" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F106" t="s">
         <v>18</v>
@@ -7330,10 +7327,10 @@
         <v>18</v>
       </c>
       <c r="H111" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="J111">
-        <v>422</v>
+        <v>200</v>
       </c>
       <c r="L111" t="s">
         <v>20</v>
@@ -7362,7 +7359,7 @@
         <v>18</v>
       </c>
       <c r="H112" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="J112">
         <v>404</v>
@@ -7394,7 +7391,7 @@
         <v>18</v>
       </c>
       <c r="H113" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="J113">
         <v>200</v>
@@ -7426,7 +7423,7 @@
         <v>18</v>
       </c>
       <c r="H114" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="J114">
         <v>500</v>
@@ -7458,7 +7455,7 @@
         <v>18</v>
       </c>
       <c r="H115" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="J115">
         <v>200</v>
@@ -7490,7 +7487,7 @@
         <v>18</v>
       </c>
       <c r="H116" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="J116">
         <v>200</v>
@@ -7522,7 +7519,7 @@
         <v>18</v>
       </c>
       <c r="H117" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="J117">
         <v>200</v>
@@ -7554,7 +7551,7 @@
         <v>18</v>
       </c>
       <c r="H118" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="J118">
         <v>404</v>
@@ -8714,7 +8711,7 @@
         <v>18</v>
       </c>
       <c r="H155" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="J155">
         <v>200</v>
@@ -9037,7 +9034,7 @@
         <v>18</v>
       </c>
       <c r="G165" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="J165">
         <v>200</v>
@@ -9211,7 +9208,7 @@
         <v>319</v>
       </c>
       <c r="C171" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D171" t="s">
         <v>44</v>
@@ -9597,7 +9594,7 @@
         <v>18</v>
       </c>
       <c r="H184" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="J184">
         <v>400</v>
@@ -10721,7 +10718,7 @@
         <v>18</v>
       </c>
       <c r="H221" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="J221">
         <v>200</v>
@@ -10753,7 +10750,7 @@
         <v>18</v>
       </c>
       <c r="H222" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="J222">
         <v>200</v>

</xml_diff>